<commit_message>
cap nhat activity diagram
</commit_message>
<xml_diff>
--- a/chuc_nang.xlsx
+++ b/chuc_nang.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_20fd\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thiet-ke-phan-mem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{0CE9A487-25B3-45FA-8C86-1A281BA7577B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71135D22-514A-47B7-8F5C-120A866F3D40}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30335406-5727-4D20-B6B2-E73A4084BA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,7 +737,7 @@
   <dimension ref="A2:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="A2:E53"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -765,7 +765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="45" customHeight="1">
       <c r="A3" s="10">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
cap nhat dac ta usecase, activity diagram
</commit_message>
<xml_diff>
--- a/chuc_nang.xlsx
+++ b/chuc_nang.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Danh sách" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -736,16 +736,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="1" max="2" width="4.875" customWidth="1"/>
+    <col min="3" max="3" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="24.375" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" s="8" customFormat="1" ht="30">

</xml_diff>

<commit_message>
cap nhat tai lieu phan tich
</commit_message>
<xml_diff>
--- a/chuc_nang.xlsx
+++ b/chuc_nang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thiet-ke-phan-mem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30335406-5727-4D20-B6B2-E73A4084BA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{30335406-5727-4D20-B6B2-E73A4084BA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DBFA1D60-6763-4007-877D-9FEA71D607B9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
     <t>Xuất báo cáo</t>
   </si>
   <si>
-    <t>tổng hợp thông tin từ 29-33 ra 1 file</t>
+    <t>tổng hợp thông tin từ 30-34 ra 1 file</t>
   </si>
   <si>
     <t>Đặt sách trước</t>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -746,6 +746,7 @@
     <col min="3" max="3" width="24.875" customWidth="1"/>
     <col min="4" max="4" width="24.375" customWidth="1"/>
     <col min="5" max="5" width="27.625" customWidth="1"/>
+    <col min="6" max="6" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" s="8" customFormat="1" ht="30">
@@ -1000,7 +1001,7 @@
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5">
       <c r="A22" s="10">
         <v>20</v>
       </c>

</xml_diff>